<commit_message>
Tv Spot evaluation Update
</commit_message>
<xml_diff>
--- a/Spot_Evaluation.xlsx
+++ b/Spot_Evaluation.xlsx
@@ -160,19 +160,19 @@
         <v>26.0</v>
       </c>
       <c r="G2" t="n">
-        <v>5.199999999999998</v>
+        <v>7.0</v>
       </c>
       <c r="H2" t="n">
         <v>32.199999999999996</v>
       </c>
       <c r="I2" t="n">
-        <v>53.240384615384635</v>
+        <v>39.550000000000004</v>
       </c>
       <c r="J2" t="n">
         <v>8.597826086956523</v>
       </c>
       <c r="K2" t="n">
-        <v>7.428571428571427</v>
+        <v>10.0</v>
       </c>
       <c r="L2" t="n">
         <v>46.0</v>
@@ -198,19 +198,19 @@
         <v>26.0</v>
       </c>
       <c r="G3" t="n">
-        <v>9.600000000000001</v>
+        <v>12.600000000000001</v>
       </c>
       <c r="H3" t="n">
         <v>72.19999999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>70.60937499999999</v>
+        <v>53.797619047619044</v>
       </c>
       <c r="J3" t="n">
         <v>9.388504155124656</v>
       </c>
       <c r="K3" t="n">
-        <v>4.000000000000001</v>
+        <v>5.250000000000001</v>
       </c>
       <c r="L3" t="n">
         <v>30.08333333333333</v>
@@ -236,19 +236,19 @@
         <v>26.0</v>
       </c>
       <c r="G4" t="n">
-        <v>8.48358208955224</v>
+        <v>9.919402985074626</v>
       </c>
       <c r="H4" t="n">
         <v>80.62686567164178</v>
       </c>
       <c r="I4" t="n">
-        <v>71.91184025334272</v>
+        <v>61.502693349383094</v>
       </c>
       <c r="J4" t="n">
         <v>7.566584598296928</v>
       </c>
       <c r="K4" t="n">
-        <v>2.12089552238806</v>
+        <v>2.4798507462686565</v>
       </c>
       <c r="L4" t="n">
         <v>20.156716417910445</v>
@@ -274,22 +274,22 @@
         <v>26.0</v>
       </c>
       <c r="G5" t="n">
-        <v>6.116417910447762</v>
+        <v>7.280597014925373</v>
       </c>
       <c r="H5" t="n">
-        <v>45.373134328358205</v>
+        <v>52.373134328358205</v>
       </c>
       <c r="I5" t="n">
-        <v>56.57886774036115</v>
+        <v>47.53181631816318</v>
       </c>
       <c r="J5" t="n">
-        <v>7.626980263157895</v>
+        <v>6.607586206896552</v>
       </c>
       <c r="K5" t="n">
-        <v>2.2653399668325043</v>
+        <v>2.6965174129353233</v>
       </c>
       <c r="L5" t="n">
-        <v>16.804864566058594</v>
+        <v>19.397457158651186</v>
       </c>
     </row>
     <row r="6">
@@ -312,22 +312,22 @@
         <v>26.0</v>
       </c>
       <c r="G6" t="n">
-        <v>10.200000000000003</v>
+        <v>11.4</v>
       </c>
       <c r="H6" t="n">
-        <v>30.4</v>
+        <v>38.2</v>
       </c>
       <c r="I6" t="n">
-        <v>39.87352941176469</v>
+        <v>35.67631578947368</v>
       </c>
       <c r="J6" t="n">
-        <v>13.378618421052632</v>
+        <v>10.646858638743455</v>
       </c>
       <c r="K6" t="n">
-        <v>6.000000000000002</v>
+        <v>6.705882352941177</v>
       </c>
       <c r="L6" t="n">
-        <v>17.88235294117647</v>
+        <v>22.47058823529412</v>
       </c>
     </row>
     <row r="7">
@@ -350,22 +350,22 @@
         <v>26.0</v>
       </c>
       <c r="G7" t="n">
-        <v>6.2</v>
+        <v>11.4</v>
       </c>
       <c r="H7" t="n">
-        <v>119.4</v>
+        <v>120.00000000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>191.3290322580645</v>
+        <v>104.05614035087719</v>
       </c>
       <c r="J7" t="n">
-        <v>9.93500837520938</v>
+        <v>9.885333333333332</v>
       </c>
       <c r="K7" t="n">
-        <v>1.2653061224489794</v>
+        <v>2.326530612244898</v>
       </c>
       <c r="L7" t="n">
-        <v>24.36734693877551</v>
+        <v>24.48979591836735</v>
       </c>
     </row>
     <row r="8">
@@ -388,22 +388,22 @@
         <v>26.0</v>
       </c>
       <c r="G8" t="n">
-        <v>7.0</v>
+        <v>11.400000000000002</v>
       </c>
       <c r="H8" t="n">
-        <v>32.0</v>
+        <v>35.400000000000006</v>
       </c>
       <c r="I8" t="n">
-        <v>48.41857142857143</v>
+        <v>29.73070175438596</v>
       </c>
       <c r="J8" t="n">
-        <v>10.5915625</v>
+        <v>9.574293785310733</v>
       </c>
       <c r="K8" t="n">
-        <v>7.0</v>
+        <v>11.400000000000002</v>
       </c>
       <c r="L8" t="n">
-        <v>32.0</v>
+        <v>35.400000000000006</v>
       </c>
     </row>
     <row r="9">
@@ -426,19 +426,19 @@
         <v>26.0</v>
       </c>
       <c r="G9" t="n">
-        <v>3.1999999999999984</v>
+        <v>12.0</v>
       </c>
       <c r="H9" t="n">
         <v>107.39999999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>476.61250000000024</v>
+        <v>127.09666666666668</v>
       </c>
       <c r="J9" t="n">
         <v>14.200744878957172</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7111111111111108</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="L9" t="n">
         <v>23.866666666666664</v>
@@ -464,22 +464,22 @@
         <v>26.0</v>
       </c>
       <c r="G10" t="n">
-        <v>3.7999999999999976</v>
+        <v>11.0</v>
       </c>
       <c r="H10" t="n">
-        <v>44.6</v>
+        <v>60.199999999999996</v>
       </c>
       <c r="I10" t="n">
-        <v>273.20526315789493</v>
+        <v>94.38000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>23.277578475336323</v>
+        <v>17.245514950166115</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7916666666666662</v>
+        <v>2.291666666666667</v>
       </c>
       <c r="L10" t="n">
-        <v>9.291666666666668</v>
+        <v>12.541666666666666</v>
       </c>
     </row>
     <row r="11">
@@ -502,22 +502,22 @@
         <v>26.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2.4000000000000017</v>
+        <v>12.2</v>
       </c>
       <c r="H11" t="n">
-        <v>108.4</v>
+        <v>112.6</v>
       </c>
       <c r="I11" t="n">
-        <v>282.43749999999983</v>
+        <v>55.56147540983607</v>
       </c>
       <c r="J11" t="n">
-        <v>6.253228782287823</v>
+        <v>6.019982238010658</v>
       </c>
       <c r="K11" t="n">
-        <v>0.5333333333333337</v>
+        <v>2.711111111111111</v>
       </c>
       <c r="L11" t="n">
-        <v>24.08888888888889</v>
+        <v>25.022222222222222</v>
       </c>
     </row>
     <row r="12">
@@ -540,19 +540,19 @@
         <v>26.0</v>
       </c>
       <c r="G12" t="n">
-        <v>29.208</v>
+        <v>31.747999999999998</v>
       </c>
       <c r="H12" t="n">
         <v>239.37</v>
       </c>
       <c r="I12" t="n">
-        <v>46.41536565324569</v>
+        <v>42.701902482046115</v>
       </c>
       <c r="J12" t="n">
         <v>5.663616994610853</v>
       </c>
       <c r="K12" t="n">
-        <v>3.357241379310345</v>
+        <v>3.6491954022988504</v>
       </c>
       <c r="L12" t="n">
         <v>27.51379310344828</v>
@@ -578,19 +578,19 @@
         <v>26.0</v>
       </c>
       <c r="G13" t="n">
-        <v>5.592000000000001</v>
+        <v>6.852</v>
       </c>
       <c r="H13" t="n">
         <v>121.63</v>
       </c>
       <c r="I13" t="n">
-        <v>123.76967095851214</v>
+        <v>101.00992410974898</v>
       </c>
       <c r="J13" t="n">
         <v>5.69037244100962</v>
       </c>
       <c r="K13" t="n">
-        <v>4.301538461538462</v>
+        <v>5.270769230769231</v>
       </c>
       <c r="L13" t="n">
         <v>93.56153846153846</v>
@@ -616,22 +616,22 @@
         <v>26.0</v>
       </c>
       <c r="G14" t="n">
-        <v>4.199999999999999</v>
+        <v>9.200000000000001</v>
       </c>
       <c r="H14" t="n">
-        <v>82.6</v>
+        <v>83.6</v>
       </c>
       <c r="I14" t="n">
-        <v>112.9761904761905</v>
+        <v>51.576086956521735</v>
       </c>
       <c r="J14" t="n">
-        <v>5.74455205811138</v>
+        <v>5.675837320574163</v>
       </c>
       <c r="K14" t="n">
-        <v>1.6799999999999997</v>
+        <v>3.6800000000000006</v>
       </c>
       <c r="L14" t="n">
-        <v>33.04</v>
+        <v>33.44</v>
       </c>
     </row>
     <row r="15">
@@ -657,19 +657,19 @@
         <v>1.0</v>
       </c>
       <c r="H15" t="n">
-        <v>3.4000000000000004</v>
+        <v>4.0</v>
       </c>
       <c r="I15" t="n">
         <v>276.85</v>
       </c>
       <c r="J15" t="n">
-        <v>81.42647058823529</v>
+        <v>69.2125</v>
       </c>
       <c r="K15" t="n">
         <v>1.25</v>
       </c>
       <c r="L15" t="n">
-        <v>4.25</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="16">
@@ -692,22 +692,22 @@
         <v>26.0</v>
       </c>
       <c r="G16" t="n">
-        <v>1.8000000000000003</v>
+        <v>2.6</v>
       </c>
       <c r="H16" t="n">
-        <v>17.8</v>
+        <v>18.0</v>
       </c>
       <c r="I16" t="n">
-        <v>150.6333333333333</v>
+        <v>104.28461538461538</v>
       </c>
       <c r="J16" t="n">
-        <v>15.23258426966292</v>
+        <v>15.063333333333333</v>
       </c>
       <c r="K16" t="n">
-        <v>3.6000000000000005</v>
+        <v>5.2</v>
       </c>
       <c r="L16" t="n">
-        <v>35.6</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="17">
@@ -733,19 +733,19 @@
         <v>7.0</v>
       </c>
       <c r="H17" t="n">
-        <v>17.799999999999997</v>
+        <v>19.2</v>
       </c>
       <c r="I17" t="n">
         <v>49.43714285714286</v>
       </c>
       <c r="J17" t="n">
-        <v>19.44157303370787</v>
+        <v>18.023958333333333</v>
       </c>
       <c r="K17" t="n">
         <v>14.0</v>
       </c>
       <c r="L17" t="n">
-        <v>35.599999999999994</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="18">
@@ -768,19 +768,19 @@
         <v>26.0</v>
       </c>
       <c r="G18" t="n">
-        <v>4.4</v>
+        <v>6.8</v>
       </c>
       <c r="H18" t="n">
         <v>56.400000000000006</v>
       </c>
       <c r="I18" t="n">
-        <v>78.64999999999999</v>
+        <v>50.891176470588235</v>
       </c>
       <c r="J18" t="n">
         <v>6.135815602836879</v>
       </c>
       <c r="K18" t="n">
-        <v>3.666666666666667</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="L18" t="n">
         <v>47.00000000000001</v>
@@ -806,22 +806,22 @@
         <v>26.0</v>
       </c>
       <c r="G19" t="n">
-        <v>3.256338028169014</v>
+        <v>7.867605633802816</v>
       </c>
       <c r="H19" t="n">
-        <v>57.4</v>
+        <v>59.4</v>
       </c>
       <c r="I19" t="n">
-        <v>156.1232266435986</v>
+        <v>64.61813462226996</v>
       </c>
       <c r="J19" t="n">
-        <v>8.856968641114982</v>
+        <v>8.558754208754209</v>
       </c>
       <c r="K19" t="n">
-        <v>2.170892018779343</v>
+        <v>5.2450704225352105</v>
       </c>
       <c r="L19" t="n">
-        <v>38.266666666666666</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="20">
@@ -844,22 +844,22 @@
         <v>26.0</v>
       </c>
       <c r="G20" t="n">
-        <v>8.200000000000001</v>
+        <v>11.8</v>
       </c>
       <c r="H20" t="n">
-        <v>95.4</v>
+        <v>98.19999999999999</v>
       </c>
       <c r="I20" t="n">
-        <v>61.998780487804865</v>
+        <v>43.083898305084745</v>
       </c>
       <c r="J20" t="n">
-        <v>5.329035639412997</v>
+        <v>5.1770875763747455</v>
       </c>
       <c r="K20" t="n">
-        <v>5.466666666666668</v>
+        <v>7.866666666666667</v>
       </c>
       <c r="L20" t="n">
-        <v>63.6</v>
+        <v>65.46666666666665</v>
       </c>
     </row>
     <row r="21">
@@ -882,22 +882,22 @@
         <v>26.0</v>
       </c>
       <c r="G21" t="n">
-        <v>-5.551115123125783E-16</v>
+        <v>4.8</v>
       </c>
       <c r="H21" t="n">
-        <v>45.8</v>
+        <v>49.400000000000006</v>
       </c>
       <c r="I21" t="n">
-        <v>-9.1583400582355456E17</v>
+        <v>105.91458333333334</v>
       </c>
       <c r="J21" t="n">
-        <v>11.100218340611354</v>
+        <v>10.291295546558702</v>
       </c>
       <c r="K21" t="n">
-        <v>-3.469446951953614E-16</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="L21" t="n">
-        <v>28.624999999999996</v>
+        <v>30.875000000000004</v>
       </c>
     </row>
     <row r="22">
@@ -920,22 +920,22 @@
         <v>26.0</v>
       </c>
       <c r="G22" t="n">
-        <v>3.2871794871794875</v>
+        <v>3.7051282051282053</v>
       </c>
       <c r="H22" t="n">
-        <v>24.199999999999996</v>
+        <v>25.799999999999997</v>
       </c>
       <c r="I22" t="n">
-        <v>154.65842433697347</v>
+        <v>137.2125259515571</v>
       </c>
       <c r="J22" t="n">
-        <v>21.007851239669424</v>
+        <v>19.705038759689923</v>
       </c>
       <c r="K22" t="n">
-        <v>3.2871794871794875</v>
+        <v>3.7051282051282053</v>
       </c>
       <c r="L22" t="n">
-        <v>24.199999999999996</v>
+        <v>25.799999999999997</v>
       </c>
     </row>
     <row r="23">
@@ -958,22 +958,22 @@
         <v>26.0</v>
       </c>
       <c r="G23" t="n">
-        <v>16.143661971830987</v>
+        <v>19.33239436619718</v>
       </c>
       <c r="H23" t="n">
-        <v>180.6</v>
+        <v>185.4</v>
       </c>
       <c r="I23" t="n">
-        <v>107.1813819577735</v>
+        <v>89.50262275972607</v>
       </c>
       <c r="J23" t="n">
-        <v>9.580841638981173</v>
+        <v>9.332793959007551</v>
       </c>
       <c r="K23" t="n">
-        <v>2.882796780684105</v>
+        <v>3.4522132796780682</v>
       </c>
       <c r="L23" t="n">
-        <v>32.25</v>
+        <v>33.10714285714286</v>
       </c>
     </row>
     <row r="24">
@@ -996,22 +996,22 @@
         <v>26.0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.8</v>
+        <v>2.0</v>
       </c>
       <c r="H24" t="n">
-        <v>15.8</v>
+        <v>18.2</v>
       </c>
       <c r="I24" t="n">
-        <v>423.66249999999997</v>
+        <v>169.465</v>
       </c>
       <c r="J24" t="n">
-        <v>21.45126582278481</v>
+        <v>18.622527472527473</v>
       </c>
       <c r="K24" t="n">
-        <v>1.142857142857143</v>
+        <v>2.857142857142857</v>
       </c>
       <c r="L24" t="n">
-        <v>22.571428571428573</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="25">
@@ -1034,22 +1034,22 @@
         <v>26.0</v>
       </c>
       <c r="G25" t="n">
-        <v>-6.8</v>
+        <v>0.6</v>
       </c>
       <c r="H25" t="n">
-        <v>10.4</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="I25" t="n">
-        <v>-49.84264705882353</v>
+        <v>564.8833333333333</v>
       </c>
       <c r="J25" t="n">
-        <v>32.589423076923076</v>
+        <v>30.26160714285714</v>
       </c>
       <c r="K25" t="n">
-        <v>-11.333333333333334</v>
+        <v>1.0</v>
       </c>
       <c r="L25" t="n">
-        <v>17.333333333333336</v>
+        <v>18.666666666666668</v>
       </c>
     </row>
     <row r="26">
@@ -1072,22 +1072,22 @@
         <v>26.0</v>
       </c>
       <c r="G26" t="n">
-        <v>7.399999999999999</v>
+        <v>9.000000000000002</v>
       </c>
       <c r="H26" t="n">
-        <v>54.0</v>
+        <v>60.60000000000001</v>
       </c>
       <c r="I26" t="n">
-        <v>84.17702702702704</v>
+        <v>69.21222222222221</v>
       </c>
       <c r="J26" t="n">
-        <v>11.53537037037037</v>
+        <v>10.279042904290428</v>
       </c>
       <c r="K26" t="n">
-        <v>2.5517241379310343</v>
+        <v>3.10344827586207</v>
       </c>
       <c r="L26" t="n">
-        <v>18.620689655172413</v>
+        <v>20.896551724137936</v>
       </c>
     </row>
     <row r="27">
@@ -1110,22 +1110,22 @@
         <v>26.0</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.5999999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="H27" t="n">
-        <v>34.6</v>
+        <v>39.6</v>
       </c>
       <c r="I27" t="n">
-        <v>-1038.1833333333336</v>
+        <v>115.35370370370369</v>
       </c>
       <c r="J27" t="n">
-        <v>18.003179190751442</v>
+        <v>15.730050505050503</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.23999999999999994</v>
+        <v>2.16</v>
       </c>
       <c r="L27" t="n">
-        <v>13.84</v>
+        <v>15.84</v>
       </c>
     </row>
     <row r="28">
@@ -1148,22 +1148,22 @@
         <v>26.0</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.2</v>
+        <v>1.0</v>
       </c>
       <c r="H28" t="n">
-        <v>19.2</v>
+        <v>21.2</v>
       </c>
       <c r="I28" t="n">
-        <v>-283.1409090909091</v>
+        <v>622.91</v>
       </c>
       <c r="J28" t="n">
-        <v>32.44322916666667</v>
+        <v>29.38254716981132</v>
       </c>
       <c r="K28" t="n">
-        <v>-1.1578947368421053</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="L28" t="n">
-        <v>10.105263157894736</v>
+        <v>11.157894736842106</v>
       </c>
     </row>
     <row r="29">
@@ -1186,22 +1186,22 @@
         <v>26.0</v>
       </c>
       <c r="G29" t="n">
-        <v>2.733016892363535</v>
+        <v>2.968644422727907</v>
       </c>
       <c r="H29" t="n">
-        <v>5.147368421052635</v>
+        <v>10.442105263157893</v>
       </c>
       <c r="I29" t="n">
-        <v>227.92028901852208</v>
+        <v>209.82977793871447</v>
       </c>
       <c r="J29" t="n">
-        <v>121.01523517382405</v>
+        <v>59.65367943548387</v>
       </c>
       <c r="K29" t="n">
-        <v>3.0366854359594835</v>
+        <v>3.298493803031008</v>
       </c>
       <c r="L29" t="n">
-        <v>5.719298245614039</v>
+        <v>11.602339181286547</v>
       </c>
     </row>
     <row r="30">
@@ -1224,22 +1224,22 @@
         <v>26.0</v>
       </c>
       <c r="G30" t="n">
-        <v>3.832007073386384</v>
+        <v>4.049955791335102</v>
       </c>
       <c r="H30" t="n">
-        <v>29.199999999999996</v>
+        <v>29.799999999999997</v>
       </c>
       <c r="I30" t="n">
-        <v>221.11389247808026</v>
+        <v>209.2146294072699</v>
       </c>
       <c r="J30" t="n">
-        <v>29.01746575342466</v>
+        <v>28.433221476510067</v>
       </c>
       <c r="K30" t="n">
-        <v>3.832007073386384</v>
+        <v>4.049955791335102</v>
       </c>
       <c r="L30" t="n">
-        <v>29.199999999999996</v>
+        <v>29.799999999999997</v>
       </c>
     </row>
     <row r="31">
@@ -1262,22 +1262,22 @@
         <v>26.0</v>
       </c>
       <c r="G31" t="n">
-        <v>1.9477965470705945</v>
+        <v>2.276271580808786</v>
       </c>
       <c r="H31" t="n">
-        <v>24.05263157894737</v>
+        <v>24.757894736842108</v>
       </c>
       <c r="I31" t="n">
-        <v>435.0094989511708</v>
+        <v>372.23589976857716</v>
       </c>
       <c r="J31" t="n">
-        <v>35.22733041575492</v>
+        <v>34.223830782312916</v>
       </c>
       <c r="K31" t="n">
-        <v>1.9477965470705945</v>
+        <v>2.276271580808786</v>
       </c>
       <c r="L31" t="n">
-        <v>24.05263157894737</v>
+        <v>24.757894736842108</v>
       </c>
     </row>
     <row r="32">
@@ -1300,22 +1300,22 @@
         <v>26.0</v>
       </c>
       <c r="G32" t="n">
-        <v>20.613953488372093</v>
+        <v>22.748837209302327</v>
       </c>
       <c r="H32" t="n">
-        <v>178.46511627906978</v>
+        <v>179.53953488372093</v>
       </c>
       <c r="I32" t="n">
-        <v>50.36297382671481</v>
+        <v>45.636618278470664</v>
       </c>
       <c r="J32" t="n">
-        <v>5.817271305707584</v>
+        <v>5.782459003652756</v>
       </c>
       <c r="K32" t="n">
-        <v>3.123326286116984</v>
+        <v>3.446793516560959</v>
       </c>
       <c r="L32" t="n">
-        <v>27.040169133192393</v>
+        <v>27.20295983086681</v>
       </c>
     </row>
     <row r="33">
@@ -1338,22 +1338,22 @@
         <v>26.0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.0</v>
+        <v>12.200000000000001</v>
       </c>
       <c r="H33" t="n">
-        <v>80.6</v>
+        <v>83.79999999999998</v>
       </c>
       <c r="I33" t="n">
-        <v>169.46333333333334</v>
+        <v>41.67131147540983</v>
       </c>
       <c r="J33" t="n">
-        <v>6.3075682382134</v>
+        <v>6.066706443914082</v>
       </c>
       <c r="K33" t="n">
-        <v>1.25</v>
+        <v>5.083333333333334</v>
       </c>
       <c r="L33" t="n">
-        <v>33.583333333333336</v>
+        <v>34.916666666666664</v>
       </c>
     </row>
     <row r="34">
@@ -1376,22 +1376,22 @@
         <v>26.0</v>
       </c>
       <c r="G34" t="n">
-        <v>21.428571428571423</v>
+        <v>24.885714285714286</v>
       </c>
       <c r="H34" t="n">
-        <v>164.54285714285712</v>
+        <v>166.34285714285713</v>
       </c>
       <c r="I34" t="n">
-        <v>50.61280000000001</v>
+        <v>43.58163030998852</v>
       </c>
       <c r="J34" t="n">
-        <v>6.591352665393298</v>
+        <v>6.520027481964961</v>
       </c>
       <c r="K34" t="n">
-        <v>5.952380952380951</v>
+        <v>6.912698412698413</v>
       </c>
       <c r="L34" t="n">
-        <v>45.706349206349195</v>
+        <v>46.2063492063492</v>
       </c>
     </row>
     <row r="35">
@@ -1414,22 +1414,22 @@
         <v>26.0</v>
       </c>
       <c r="G35" t="n">
-        <v>17.7273132664437</v>
+        <v>20.17079152731327</v>
       </c>
       <c r="H35" t="n">
-        <v>133.8</v>
+        <v>136.0</v>
       </c>
       <c r="I35" t="n">
-        <v>68.8276887569648</v>
+        <v>60.48994152499281</v>
       </c>
       <c r="J35" t="n">
-        <v>9.119058295964125</v>
+        <v>8.97154411764706</v>
       </c>
       <c r="K35" t="n">
-        <v>4.220788872962786</v>
+        <v>4.802569411265064</v>
       </c>
       <c r="L35" t="n">
-        <v>31.857142857142858</v>
+        <v>32.38095238095238</v>
       </c>
     </row>
     <row r="36">
@@ -1452,22 +1452,22 @@
         <v>26.0</v>
       </c>
       <c r="G36" t="n">
-        <v>6.386046511627907</v>
+        <v>7.4511627906976745</v>
       </c>
       <c r="H36" t="n">
-        <v>78.53488372093022</v>
+        <v>78.86046511627907</v>
       </c>
       <c r="I36" t="n">
-        <v>86.70466132556447</v>
+        <v>74.31054931335831</v>
       </c>
       <c r="J36" t="n">
-        <v>7.050370151021618</v>
+        <v>7.02126216455323</v>
       </c>
       <c r="K36" t="n">
-        <v>3.1930232558139533</v>
+        <v>3.7255813953488373</v>
       </c>
       <c r="L36" t="n">
-        <v>39.26744186046511</v>
+        <v>39.43023255813954</v>
       </c>
     </row>
     <row r="37">
@@ -1490,22 +1490,22 @@
         <v>26.0</v>
       </c>
       <c r="G37" t="n">
-        <v>13.571428571428571</v>
+        <v>15.714285714285714</v>
       </c>
       <c r="H37" t="n">
-        <v>76.85714285714286</v>
+        <v>85.45714285714286</v>
       </c>
       <c r="I37" t="n">
-        <v>74.92063157894736</v>
+        <v>64.70418181818182</v>
       </c>
       <c r="J37" t="n">
-        <v>13.229479553903344</v>
+        <v>11.898127716482781</v>
       </c>
       <c r="K37" t="n">
-        <v>5.026455026455026</v>
+        <v>5.82010582010582</v>
       </c>
       <c r="L37" t="n">
-        <v>28.465608465608465</v>
+        <v>31.65079365079365</v>
       </c>
     </row>
     <row r="38">
@@ -1528,22 +1528,22 @@
         <v>26.0</v>
       </c>
       <c r="G38" t="n">
-        <v>19.981128205128204</v>
+        <v>20.365128205128205</v>
       </c>
       <c r="H38" t="n">
-        <v>91.49600000000001</v>
+        <v>93.46400000000001</v>
       </c>
       <c r="I38" t="n">
-        <v>50.88701646681997</v>
+        <v>49.92750302175665</v>
       </c>
       <c r="J38" t="n">
-        <v>11.112835533793826</v>
+        <v>10.878841051099887</v>
       </c>
       <c r="K38" t="n">
-        <v>4.162735042735043</v>
+        <v>4.242735042735043</v>
       </c>
       <c r="L38" t="n">
-        <v>19.06166666666667</v>
+        <v>19.47166666666667</v>
       </c>
     </row>
     <row r="39">
@@ -1566,19 +1566,19 @@
         <v>26.0</v>
       </c>
       <c r="G39" t="n">
-        <v>28.799999999999994</v>
+        <v>36.0</v>
       </c>
       <c r="H39" t="n">
         <v>389.79999999999995</v>
       </c>
       <c r="I39" t="n">
-        <v>115.35347222222224</v>
+        <v>92.28277777777777</v>
       </c>
       <c r="J39" t="n">
         <v>8.522780913288866</v>
       </c>
       <c r="K39" t="n">
-        <v>2.2325581395348832</v>
+        <v>2.7906976744186047</v>
       </c>
       <c r="L39" t="n">
         <v>30.21705426356589</v>
@@ -1604,22 +1604,22 @@
         <v>26.0</v>
       </c>
       <c r="G40" t="n">
-        <v>12.491558528428094</v>
+        <v>12.864080267558528</v>
       </c>
       <c r="H40" t="n">
-        <v>80.70400000000001</v>
+        <v>82.336</v>
       </c>
       <c r="I40" t="n">
-        <v>70.544439910725</v>
+        <v>68.5015937145769</v>
       </c>
       <c r="J40" t="n">
-        <v>10.919037470261696</v>
+        <v>10.70260882238632</v>
       </c>
       <c r="K40" t="n">
-        <v>4.626503158677071</v>
+        <v>4.764474173169825</v>
       </c>
       <c r="L40" t="n">
-        <v>29.89037037037037</v>
+        <v>30.494814814814813</v>
       </c>
     </row>
     <row r="41">
@@ -1642,22 +1642,22 @@
         <v>26.0</v>
       </c>
       <c r="G41" t="n">
-        <v>14.600000000000003</v>
+        <v>21.2</v>
       </c>
       <c r="H41" t="n">
-        <v>151.4</v>
+        <v>157.8</v>
       </c>
       <c r="I41" t="n">
-        <v>4.104109589041095</v>
+        <v>2.8264150943396227</v>
       </c>
       <c r="J41" t="n">
-        <v>0.39577278731836196</v>
+        <v>0.3797211660329531</v>
       </c>
       <c r="K41" t="n">
-        <v>3.1739130434782616</v>
+        <v>4.608695652173913</v>
       </c>
       <c r="L41" t="n">
-        <v>32.913043478260875</v>
+        <v>34.30434782608696</v>
       </c>
     </row>
     <row r="42">
@@ -1680,22 +1680,22 @@
         <v>26.0</v>
       </c>
       <c r="G42" t="n">
-        <v>8.8</v>
+        <v>14.6</v>
       </c>
       <c r="H42" t="n">
-        <v>62.0</v>
+        <v>67.0</v>
       </c>
       <c r="I42" t="n">
-        <v>86.51477272727273</v>
+        <v>52.145890410958906</v>
       </c>
       <c r="J42" t="n">
-        <v>12.279516129032258</v>
+        <v>11.363134328358209</v>
       </c>
       <c r="K42" t="n">
-        <v>4.0</v>
+        <v>6.636363636363636</v>
       </c>
       <c r="L42" t="n">
-        <v>28.18181818181818</v>
+        <v>30.454545454545453</v>
       </c>
     </row>
     <row r="43">
@@ -1718,22 +1718,22 @@
         <v>26.0</v>
       </c>
       <c r="G43" t="n">
-        <v>10.799999999999997</v>
+        <v>14.200000000000001</v>
       </c>
       <c r="H43" t="n">
-        <v>26.200000000000003</v>
+        <v>35.800000000000004</v>
       </c>
       <c r="I43" t="n">
-        <v>5.911111111111113</v>
+        <v>4.495774647887324</v>
       </c>
       <c r="J43" t="n">
-        <v>2.4366412213740456</v>
+        <v>1.783240223463687</v>
       </c>
       <c r="K43" t="n">
-        <v>6.352941176470587</v>
+        <v>8.352941176470589</v>
       </c>
       <c r="L43" t="n">
-        <v>15.411764705882355</v>
+        <v>21.058823529411768</v>
       </c>
     </row>
     <row r="44">
@@ -1756,19 +1756,19 @@
         <v>26.0</v>
       </c>
       <c r="G44" t="n">
-        <v>38.599999999999994</v>
+        <v>41.0</v>
       </c>
       <c r="H44" t="n">
         <v>420.6</v>
       </c>
       <c r="I44" t="n">
-        <v>127.31632124352333</v>
+        <v>119.86365853658536</v>
       </c>
       <c r="J44" t="n">
         <v>11.684284355682358</v>
       </c>
       <c r="K44" t="n">
-        <v>2.6081081081081074</v>
+        <v>2.77027027027027</v>
       </c>
       <c r="L44" t="n">
         <v>28.41891891891892</v>
@@ -1794,22 +1794,22 @@
         <v>26.0</v>
       </c>
       <c r="G45" t="n">
-        <v>11.200000000000003</v>
+        <v>18.599999999999998</v>
       </c>
       <c r="H45" t="n">
-        <v>126.0</v>
+        <v>137.4</v>
       </c>
       <c r="I45" t="n">
-        <v>287.48124999999993</v>
+        <v>173.10698924731184</v>
       </c>
       <c r="J45" t="n">
-        <v>25.55388888888889</v>
+        <v>23.433697234352255</v>
       </c>
       <c r="K45" t="n">
-        <v>1.8064516129032262</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="L45" t="n">
-        <v>20.32258064516129</v>
+        <v>22.161290322580644</v>
       </c>
     </row>
     <row r="46">
@@ -1832,22 +1832,22 @@
         <v>26.0</v>
       </c>
       <c r="G46" t="n">
-        <v>4.399999999999999</v>
+        <v>12.200000000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>95.80000000000001</v>
+        <v>96.80000000000001</v>
       </c>
       <c r="I46" t="n">
-        <v>231.0863636363637</v>
+        <v>83.34262295081966</v>
       </c>
       <c r="J46" t="n">
-        <v>10.613569937369519</v>
+        <v>10.503925619834709</v>
       </c>
       <c r="K46" t="n">
-        <v>1.4193548387096768</v>
+        <v>3.935483870967742</v>
       </c>
       <c r="L46" t="n">
-        <v>30.903225806451616</v>
+        <v>31.225806451612907</v>
       </c>
     </row>
     <row r="47">
@@ -1870,19 +1870,19 @@
         <v>26.0</v>
       </c>
       <c r="G47" t="n">
-        <v>24.290909090909093</v>
+        <v>28.33846153846154</v>
       </c>
       <c r="H47" t="n">
         <v>338.2657342657343</v>
       </c>
       <c r="I47" t="n">
-        <v>136.76639221556886</v>
+        <v>117.23219326818673</v>
       </c>
       <c r="J47" t="n">
         <v>9.82121351194906</v>
       </c>
       <c r="K47" t="n">
-        <v>2.1122529644268777</v>
+        <v>2.4642140468227427</v>
       </c>
       <c r="L47" t="n">
         <v>29.414411675281244</v>
@@ -1908,22 +1908,22 @@
         <v>26.0</v>
       </c>
       <c r="G48" t="n">
-        <v>6.309090909090908</v>
+        <v>9.061538461538461</v>
       </c>
       <c r="H48" t="n">
-        <v>78.73426573426573</v>
+        <v>82.33426573426573</v>
       </c>
       <c r="I48" t="n">
-        <v>118.1834293948127</v>
+        <v>82.2851443123939</v>
       </c>
       <c r="J48" t="n">
-        <v>9.470209610089706</v>
+        <v>9.056132259763205</v>
       </c>
       <c r="K48" t="n">
-        <v>2.253246753246753</v>
+        <v>3.2362637362637363</v>
       </c>
       <c r="L48" t="n">
-        <v>28.11938061938062</v>
+        <v>29.405094905094906</v>
       </c>
     </row>
     <row r="49">
@@ -1946,19 +1946,19 @@
         <v>26.0</v>
       </c>
       <c r="G49" t="n">
-        <v>7.0</v>
+        <v>10.999999999999998</v>
       </c>
       <c r="H49" t="n">
         <v>69.19999999999999</v>
       </c>
       <c r="I49" t="n">
-        <v>116.20285714285714</v>
+        <v>73.94727272727273</v>
       </c>
       <c r="J49" t="n">
         <v>11.75462427745665</v>
       </c>
       <c r="K49" t="n">
-        <v>1.627906976744186</v>
+        <v>2.5581395348837206</v>
       </c>
       <c r="L49" t="n">
         <v>16.09302325581395</v>
@@ -1984,19 +1984,19 @@
         <v>26.0</v>
       </c>
       <c r="G50" t="n">
-        <v>14.399999999999999</v>
+        <v>15.2</v>
       </c>
       <c r="H50" t="n">
         <v>78.0</v>
       </c>
       <c r="I50" t="n">
-        <v>141.21875</v>
+        <v>133.78618421052633</v>
       </c>
       <c r="J50" t="n">
         <v>26.071153846153845</v>
       </c>
       <c r="K50" t="n">
-        <v>3.130434782608696</v>
+        <v>3.3043478260869565</v>
       </c>
       <c r="L50" t="n">
         <v>16.956521739130437</v>
@@ -2022,22 +2022,22 @@
         <v>26.0</v>
       </c>
       <c r="G51" t="n">
-        <v>-2.1999999999999997</v>
+        <v>9.4</v>
       </c>
       <c r="H51" t="n">
-        <v>7.2</v>
+        <v>21.0</v>
       </c>
       <c r="I51" t="n">
-        <v>-346.05909090909097</v>
+        <v>80.99255319148936</v>
       </c>
       <c r="J51" t="n">
-        <v>105.74027777777778</v>
+        <v>36.25380952380952</v>
       </c>
       <c r="K51" t="n">
-        <v>-1.4666666666666666</v>
+        <v>6.266666666666667</v>
       </c>
       <c r="L51" t="n">
-        <v>4.8</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="52">
@@ -2060,22 +2060,22 @@
         <v>26.0</v>
       </c>
       <c r="G52" t="n">
-        <v>18.45714285714286</v>
+        <v>22.714285714285715</v>
       </c>
       <c r="H52" t="n">
-        <v>211.2</v>
+        <v>215.39999999999998</v>
       </c>
       <c r="I52" t="n">
-        <v>211.1724458204334</v>
+        <v>171.59421383647796</v>
       </c>
       <c r="J52" t="n">
-        <v>18.45473484848485</v>
+        <v>18.09489322191272</v>
       </c>
       <c r="K52" t="n">
-        <v>1.619047619047619</v>
+        <v>1.9924812030075187</v>
       </c>
       <c r="L52" t="n">
-        <v>18.52631578947368</v>
+        <v>18.89473684210526</v>
       </c>
     </row>
     <row r="53">
@@ -2098,22 +2098,22 @@
         <v>26.0</v>
       </c>
       <c r="G53" t="n">
-        <v>22.400000000000002</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="H53" t="n">
-        <v>141.0</v>
+        <v>147.0</v>
       </c>
       <c r="I53" t="n">
-        <v>3.7499999999999996</v>
+        <v>3.471074380165289</v>
       </c>
       <c r="J53" t="n">
-        <v>0.5957446808510638</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="K53" t="n">
-        <v>3.612903225806452</v>
+        <v>3.9032258064516134</v>
       </c>
       <c r="L53" t="n">
-        <v>22.741935483870968</v>
+        <v>23.709677419354836</v>
       </c>
     </row>
     <row r="54">
@@ -2136,22 +2136,22 @@
         <v>26.0</v>
       </c>
       <c r="G54" t="n">
-        <v>2.7428571428571424</v>
+        <v>8.285714285714285</v>
       </c>
       <c r="H54" t="n">
-        <v>40.400000000000006</v>
+        <v>43.800000000000004</v>
       </c>
       <c r="I54" t="n">
-        <v>277.5682291666667</v>
+        <v>91.88465517241382</v>
       </c>
       <c r="J54" t="n">
-        <v>18.844801980198017</v>
+        <v>17.381963470319633</v>
       </c>
       <c r="K54" t="n">
-        <v>1.443609022556391</v>
+        <v>4.360902255639098</v>
       </c>
       <c r="L54" t="n">
-        <v>21.263157894736846</v>
+        <v>23.052631578947373</v>
       </c>
     </row>
     <row r="55">
@@ -2174,22 +2174,22 @@
         <v>26.0</v>
       </c>
       <c r="G55" t="n">
-        <v>7.0</v>
+        <v>11.199999999999998</v>
       </c>
       <c r="H55" t="n">
-        <v>93.0</v>
+        <v>96.80000000000001</v>
       </c>
       <c r="I55" t="n">
-        <v>242.09</v>
+        <v>151.30625000000003</v>
       </c>
       <c r="J55" t="n">
-        <v>18.221827956989248</v>
+        <v>17.50650826446281</v>
       </c>
       <c r="K55" t="n">
-        <v>1.1475409836065575</v>
+        <v>1.8360655737704914</v>
       </c>
       <c r="L55" t="n">
-        <v>15.245901639344263</v>
+        <v>15.868852459016397</v>
       </c>
     </row>
     <row r="56">
@@ -2212,22 +2212,22 @@
         <v>26.0</v>
       </c>
       <c r="G56" t="n">
-        <v>-9.399999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="H56" t="n">
-        <v>56.0</v>
+        <v>64.2</v>
       </c>
       <c r="I56" t="n">
-        <v>-58.90425531914895</v>
+        <v>102.53703703703704</v>
       </c>
       <c r="J56" t="n">
-        <v>9.887500000000001</v>
+        <v>8.624610591900312</v>
       </c>
       <c r="K56" t="n">
-        <v>-5.529411764705881</v>
+        <v>3.1764705882352944</v>
       </c>
       <c r="L56" t="n">
-        <v>32.94117647058824</v>
+        <v>37.76470588235294</v>
       </c>
     </row>
     <row r="57">
@@ -2250,22 +2250,22 @@
         <v>26.0</v>
       </c>
       <c r="G57" t="n">
-        <v>11.267605633802818</v>
+        <v>13.273239436619717</v>
       </c>
       <c r="H57" t="n">
-        <v>79.09859154929578</v>
+        <v>80.92112676056338</v>
       </c>
       <c r="I57" t="n">
-        <v>90.23922499999999</v>
+        <v>76.60375636672327</v>
       </c>
       <c r="J57" t="n">
-        <v>12.854590455840455</v>
+        <v>12.565074668430396</v>
       </c>
       <c r="K57" t="n">
-        <v>3.314001657000829</v>
+        <v>3.9038939519469755</v>
       </c>
       <c r="L57" t="n">
-        <v>23.264291632145817</v>
+        <v>23.8003314001657</v>
       </c>
     </row>
     <row r="58">
@@ -2288,22 +2288,22 @@
         <v>26.0</v>
       </c>
       <c r="G58" t="n">
-        <v>23.732394366197184</v>
+        <v>28.12676056338028</v>
       </c>
       <c r="H58" t="n">
-        <v>265.10140845070424</v>
+        <v>267.07887323943663</v>
       </c>
       <c r="I58" t="n">
-        <v>116.6540534124629</v>
+        <v>98.42868302453681</v>
       </c>
       <c r="J58" t="n">
-        <v>10.443098043799342</v>
+        <v>10.365776844947423</v>
       </c>
       <c r="K58" t="n">
-        <v>2.1974439227960354</v>
+        <v>2.60432968179447</v>
       </c>
       <c r="L58" t="n">
-        <v>24.54642670839854</v>
+        <v>24.729525299947834</v>
       </c>
     </row>
     <row r="59">
@@ -2326,22 +2326,22 @@
         <v>26.0</v>
       </c>
       <c r="G59" t="n">
-        <v>3.3999999999999977</v>
+        <v>11.8</v>
       </c>
       <c r="H59" t="n">
-        <v>69.19999999999999</v>
+        <v>77.99999999999999</v>
       </c>
       <c r="I59" t="n">
-        <v>219.30294117647074</v>
+        <v>63.188983050847455</v>
       </c>
       <c r="J59" t="n">
-        <v>10.775000000000002</v>
+        <v>9.559358974358975</v>
       </c>
       <c r="K59" t="n">
-        <v>1.6999999999999988</v>
+        <v>5.9</v>
       </c>
       <c r="L59" t="n">
-        <v>34.599999999999994</v>
+        <v>38.99999999999999</v>
       </c>
     </row>
     <row r="60">
@@ -2364,22 +2364,22 @@
         <v>26.0</v>
       </c>
       <c r="G60" t="n">
-        <v>14.0</v>
+        <v>21.2</v>
       </c>
       <c r="H60" t="n">
-        <v>88.4</v>
+        <v>90.80000000000001</v>
       </c>
       <c r="I60" t="n">
-        <v>169.46214285714285</v>
+        <v>111.90896226415094</v>
       </c>
       <c r="J60" t="n">
-        <v>26.837895927601807</v>
+        <v>26.128524229074884</v>
       </c>
       <c r="K60" t="n">
-        <v>2.2222222222222223</v>
+        <v>3.365079365079365</v>
       </c>
       <c r="L60" t="n">
-        <v>14.031746031746033</v>
+        <v>14.412698412698415</v>
       </c>
     </row>
     <row r="61">
@@ -2402,22 +2402,22 @@
         <v>26.0</v>
       </c>
       <c r="G61" t="n">
-        <v>14.689473684210526</v>
+        <v>17.821052631578944</v>
       </c>
       <c r="H61" t="n">
-        <v>64.11578947368422</v>
+        <v>69.36842105263159</v>
       </c>
       <c r="I61" t="n">
-        <v>5.718380508778216</v>
+        <v>4.713526284701714</v>
       </c>
       <c r="J61" t="n">
-        <v>1.3101296995567229</v>
+        <v>1.21092564491654</v>
       </c>
       <c r="K61" t="n">
-        <v>2.7202729044834304</v>
+        <v>3.3001949317738783</v>
       </c>
       <c r="L61" t="n">
-        <v>11.873294346978557</v>
+        <v>12.846003898635479</v>
       </c>
     </row>
     <row r="62">
@@ -2440,22 +2440,22 @@
         <v>26.0</v>
       </c>
       <c r="G62" t="n">
-        <v>7.200000000000001</v>
+        <v>12.600000000000001</v>
       </c>
       <c r="H62" t="n">
-        <v>66.4</v>
+        <v>68.6</v>
       </c>
       <c r="I62" t="n">
-        <v>8.322222222222221</v>
+        <v>4.7555555555555555</v>
       </c>
       <c r="J62" t="n">
-        <v>0.9024096385542169</v>
+        <v>0.8734693877551022</v>
       </c>
       <c r="K62" t="n">
-        <v>2.3225806451612905</v>
+        <v>4.064516129032258</v>
       </c>
       <c r="L62" t="n">
-        <v>21.41935483870968</v>
+        <v>22.129032258064512</v>
       </c>
     </row>
     <row r="63">
@@ -2478,22 +2478,22 @@
         <v>26.0</v>
       </c>
       <c r="G63" t="n">
-        <v>0.0</v>
+        <v>7.2</v>
       </c>
       <c r="H63" t="n">
-        <v>113.4</v>
-      </c>
-      <c r="I63" t="e">
-        <v>#DIV/0!</v>
+        <v>116.4</v>
+      </c>
+      <c r="I63" t="n">
+        <v>122.39027777777778</v>
       </c>
       <c r="J63" t="n">
-        <v>7.7708112874779545</v>
+        <v>7.57053264604811</v>
       </c>
       <c r="K63" t="n">
-        <v>0.0</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="L63" t="n">
-        <v>40.50000000000001</v>
+        <v>41.57142857142858</v>
       </c>
     </row>
     <row r="64">
@@ -2516,22 +2516,22 @@
         <v>26.0</v>
       </c>
       <c r="G64" t="n">
-        <v>6.710526315789475</v>
+        <v>8.978947368421053</v>
       </c>
       <c r="H64" t="n">
-        <v>58.68421052631579</v>
+        <v>59.03157894736842</v>
       </c>
       <c r="I64" t="n">
-        <v>113.45309803921566</v>
+        <v>84.79056271981243</v>
       </c>
       <c r="J64" t="n">
-        <v>12.973336322869956</v>
+        <v>12.896995363766049</v>
       </c>
       <c r="K64" t="n">
-        <v>3.0502392344497613</v>
+        <v>4.08133971291866</v>
       </c>
       <c r="L64" t="n">
-        <v>26.674641148325357</v>
+        <v>26.832535885167463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>